<commit_message>
Atualizando meios de saida
</commit_message>
<xml_diff>
--- a/relatorio.xlsx
+++ b/relatorio.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Data</t>
   </si>
@@ -64,34 +64,40 @@
     <t>Ultima Prestação</t>
   </si>
   <si>
-    <t>14/02/2023</t>
-  </si>
-  <si>
-    <t>15:33</t>
+    <t>27/02/2023</t>
+  </si>
+  <si>
+    <t>07:57</t>
   </si>
   <si>
     <t>Guilherme</t>
   </si>
   <si>
-    <t>R$ 4.193.328,49</t>
+    <t>R$ 7.152.446,82</t>
+  </si>
+  <si>
+    <t>R$ 28,00</t>
   </si>
   <si>
     <t>R$ 0,00</t>
   </si>
   <si>
-    <t>2023-02-12 23:59:44</t>
-  </si>
-  <si>
-    <t>2023-02-10 00:00:00</t>
+    <t>R$ 7.152.474,82</t>
+  </si>
+  <si>
+    <t>2023-02-25 23:59:41</t>
+  </si>
+  <si>
+    <t>2023-02-22 00:00:00</t>
   </si>
   <si>
     <t>2023-02-03 11:50:27.167000</t>
   </si>
   <si>
-    <t>2023-02-06 11:10:56.400000</t>
-  </si>
-  <si>
-    <t>12/02/2023</t>
+    <t>2023-02-24 16:02:26.523000</t>
+  </si>
+  <si>
+    <t>Não há registros a serem exibidos.</t>
   </si>
 </sst>
 </file>
@@ -516,13 +522,13 @@
         <v>18</v>
       </c>
       <c r="D2">
-        <v>52837</v>
+        <v>88359</v>
       </c>
       <c r="E2">
-        <v>52837</v>
+        <v>88358</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -534,25 +540,25 @@
         <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>